<commit_message>
Loads of modelling and a bit of python
</commit_message>
<xml_diff>
--- a/experiment02/Results2.xlsx
+++ b/experiment02/Results2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gibbens\Documents\Arduino\EyeBolt\experiment02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFD1DF-D3F5-4D45-85C0-A260F554F1F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81EC567-2647-4B5B-90BC-A499628FA370}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{08EADBEC-E985-487F-AAB7-8862C9937860}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{08EADBEC-E985-487F-AAB7-8862C9937860}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -8711,6 +8711,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Single</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> 360 degree s</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>can</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> paths for T-shaped block</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14300,7 +14338,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9A748435-012D-4F5F-A554-49A045A23A5F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14771,7 +14809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B72296B-B747-4D5C-AF42-F672145DDD36}">
   <dimension ref="A1:AA201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>

</xml_diff>